<commit_message>
Added data from 2024-08-24 - 2024-09-07.
</commit_message>
<xml_diff>
--- a/data/Floor=2/Location=Unit 210/Device=03/M10+_device03_08-24-2024 14:08:34.xlsx
+++ b/data/Floor=2/Location=Unit 210/Device=03/M10+_device03_08-24-2024 14:08:34.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jack/Developer/Personal/Trellis Air Quality/trellis-aq/data/Floor=2/Location=Unit 210/Device=03/M10+_device03_08-24-2024 14:08:"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59B436F-D9F5-A147-8B78-45F1F053F3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="17160" yWindow="6360" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NO." sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -412,8 +418,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,13 +466,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -504,7 +518,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -538,6 +552,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -572,9 +587,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -747,14 +763,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -780,7 +808,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -806,7 +834,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -832,7 +860,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -858,7 +886,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -884,7 +912,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -910,7 +938,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -936,7 +964,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -962,7 +990,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -988,7 +1016,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1014,7 +1042,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1040,7 +1068,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1066,7 +1094,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1092,7 +1120,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1118,7 +1146,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -1144,7 +1172,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -1170,7 +1198,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -1196,7 +1224,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -1222,7 +1250,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
@@ -1248,7 +1276,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
@@ -1274,7 +1302,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
@@ -1300,7 +1328,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
@@ -1326,7 +1354,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>60</v>
       </c>
@@ -1352,7 +1380,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
@@ -1378,7 +1406,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>65</v>
       </c>

</xml_diff>